<commit_message>
Update Portuguese Excel file
</commit_message>
<xml_diff>
--- a/ErgoLux/localization/Portuguese (pt-BR) translation.xlsx
+++ b/ErgoLux/localization/Portuguese (pt-BR) translation.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44993843R\source\repos\ErgoLux\ErgoLux\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B91E14-CB26-4727-848D-AF3BDFC3DB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB1AB9-84B5-426A-A94F-177A15332539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
   <sheets>
-    <sheet name="pt-PT" sheetId="2" r:id="rId1"/>
+    <sheet name="pt-BR" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1230,7 +1230,7 @@
     <t>milliseconds, millisecond, milliseconds</t>
   </si>
   <si>
-    <t>Portuguese (pt-PT)</t>
+    <t>Portuguese (pt-BR)</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1330,7 @@
     <tableColumn id="1" xr3:uid="{15B209E7-880B-40F3-8D04-E1E0C18F3997}" name="Key" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{1492BE55-1C7C-4C02-9979-85AD6633F924}" name="Comment" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{3A0B826D-ACD0-42A2-BC11-CDF70F40C5E5}" name="English" dataDxfId="1"/>
-    <tableColumn id="31" xr3:uid="{482B5252-4A88-4C9D-8D6A-67323FB06C35}" name="Portuguese (pt-PT)" dataDxfId="0"/>
+    <tableColumn id="31" xr3:uid="{482B5252-4A88-4C9D-8D6A-67323FB06C35}" name="Portuguese (pt-BR)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>